<commit_message>
Actualización de datos, densidad del árbol agregado en datos y ordenar
</commit_message>
<xml_diff>
--- a/datos/Captura_Info.xlsx
+++ b/datos/Captura_Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayman El Salous Mnz\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184FB4F3-711E-4704-81D6-C50132455767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E678496D-2B92-4C2A-91CB-2E82D408B0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{20B9D2B3-C467-4B2A-8955-CEFACBBCABD7}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Ecosis. Salida 2" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ecosis. Salida 2'!$B$2:$G$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ecosis. Salida 2'!$B$2:$H$127</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="51">
   <si>
     <t>Site</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Circumference_(cm)</t>
+  </si>
+  <si>
+    <t>Wood_density_(g_cm^-3)</t>
   </si>
   <si>
     <t>Pseudalbizzia multiflora</t>
@@ -290,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -313,10 +316,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -331,7 +340,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -668,7 +677,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C545A6F-2989-4DB9-8EDF-13C16FDF8F37}">
-  <dimension ref="B1:V127"/>
+  <dimension ref="B1:W127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -681,11 +690,12 @@
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="42.28515625" customWidth="1"/>
     <col min="7" max="7" width="33.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="33.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:23" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -704,9 +714,12 @@
       <c r="G2" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="H2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="4">
@@ -724,9 +737,12 @@
       <c r="G3" s="7">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="H3" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="4">
@@ -744,9 +760,12 @@
       <c r="G4" s="7">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="10" t="s">
+      <c r="H4" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="4">
@@ -764,15 +783,18 @@
       <c r="G5" s="7">
         <v>48</v>
       </c>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-    </row>
-    <row r="6" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="10" t="s">
+      <c r="H5" s="8">
+        <v>0.59</v>
+      </c>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+    </row>
+    <row r="6" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="4">
@@ -790,15 +812,18 @@
       <c r="G6" s="7">
         <v>62</v>
       </c>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
-    </row>
-    <row r="7" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="10" t="s">
+      <c r="H6" s="8">
+        <v>0.59</v>
+      </c>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+    </row>
+    <row r="7" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="4">
@@ -816,15 +841,18 @@
       <c r="G7" s="7">
         <v>49</v>
       </c>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-    </row>
-    <row r="8" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="10" t="s">
+      <c r="H7" s="8">
+        <v>0.59</v>
+      </c>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+    </row>
+    <row r="8" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="4">
@@ -842,21 +870,24 @@
       <c r="G8" s="7">
         <v>70</v>
       </c>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-    </row>
-    <row r="9" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="10" t="s">
+      <c r="H8" s="8">
+        <v>0.59</v>
+      </c>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+    </row>
+    <row r="9" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="6">
@@ -868,15 +899,18 @@
       <c r="G9" s="7">
         <v>16</v>
       </c>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-    </row>
-    <row r="10" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="H9" s="8">
+        <v>0.69</v>
+      </c>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+    </row>
+    <row r="10" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="4">
@@ -894,9 +928,12 @@
       <c r="G10" s="7">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="H10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="4">
@@ -914,9 +951,12 @@
       <c r="G11" s="7">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="H11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="4">
@@ -934,9 +974,12 @@
       <c r="G12" s="7">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+      <c r="H12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="4">
@@ -954,9 +997,12 @@
       <c r="G13" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+      <c r="H13" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="4">
@@ -974,9 +1020,12 @@
       <c r="G14" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+      <c r="H14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="4">
@@ -994,9 +1043,12 @@
       <c r="G15" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+      <c r="H15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="4">
@@ -1014,9 +1066,12 @@
       <c r="G16" s="7">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="H16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="4">
@@ -1034,9 +1089,12 @@
       <c r="G17" s="7">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="10" t="s">
+      <c r="H17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="4">
@@ -1054,9 +1112,12 @@
       <c r="G18" s="7">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="H18" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="4">
@@ -1074,9 +1135,12 @@
       <c r="G19" s="7">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
+      <c r="H19" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="4">
@@ -1094,9 +1158,12 @@
       <c r="G20" s="7">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
+      <c r="H20" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="4">
@@ -1114,9 +1181,12 @@
       <c r="G21" s="7">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
+      <c r="H21" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="4">
@@ -1134,9 +1204,12 @@
       <c r="G22" s="7">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
+      <c r="H22" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="4">
@@ -1154,9 +1227,12 @@
       <c r="G23" s="7">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
+      <c r="H23" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="4">
@@ -1174,9 +1250,12 @@
       <c r="G24" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
+      <c r="H24" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="4">
@@ -1194,9 +1273,12 @@
       <c r="G25" s="7">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
+      <c r="H25" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="4">
@@ -1214,9 +1296,12 @@
       <c r="G26" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="10" t="s">
+      <c r="H26" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="4">
@@ -1234,9 +1319,12 @@
       <c r="G27" s="7">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
+      <c r="H27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="4">
@@ -1254,9 +1342,12 @@
       <c r="G28" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
+      <c r="H28" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="4">
@@ -1274,612 +1365,705 @@
       <c r="G29" s="7">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="10" t="s">
+      <c r="H29" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="4">
         <v>1</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="9">
-        <v>0</v>
-      </c>
-      <c r="F30" s="9">
+      <c r="E30" s="10">
+        <v>0</v>
+      </c>
+      <c r="F30" s="10">
         <v>0</v>
       </c>
       <c r="G30" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="10" t="s">
+      <c r="H30" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="4">
         <v>1</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="9">
-        <v>0</v>
-      </c>
-      <c r="F31" s="9">
+      <c r="E31" s="10">
+        <v>0</v>
+      </c>
+      <c r="F31" s="10">
         <v>0</v>
       </c>
       <c r="G31" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="10" t="s">
+      <c r="H31" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="4">
         <v>1</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="9">
-        <v>0</v>
-      </c>
-      <c r="F32" s="9">
+      <c r="E32" s="10">
+        <v>0</v>
+      </c>
+      <c r="F32" s="10">
         <v>0</v>
       </c>
       <c r="G32" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="10" t="s">
+      <c r="H32" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="4">
         <v>1</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="9">
-        <v>0</v>
-      </c>
-      <c r="F33" s="9">
+      <c r="E33" s="10">
+        <v>0</v>
+      </c>
+      <c r="F33" s="10">
         <v>0</v>
       </c>
       <c r="G33" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="10" t="s">
+      <c r="H33" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="4">
         <v>1</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="9">
-        <v>0</v>
-      </c>
-      <c r="F34" s="9">
+      <c r="E34" s="10">
+        <v>0</v>
+      </c>
+      <c r="F34" s="10">
         <v>0</v>
       </c>
       <c r="G34" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="10" t="s">
+      <c r="H34" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="4">
         <v>1</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="9">
-        <v>0</v>
-      </c>
-      <c r="F35" s="9">
+      <c r="E35" s="10">
+        <v>0</v>
+      </c>
+      <c r="F35" s="10">
         <v>0</v>
       </c>
       <c r="G35" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="10" t="s">
+      <c r="H35" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="4">
         <v>1</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="9">
-        <v>0</v>
-      </c>
-      <c r="F36" s="9">
+      <c r="E36" s="10">
+        <v>0</v>
+      </c>
+      <c r="F36" s="10">
         <v>0</v>
       </c>
       <c r="G36" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="10" t="s">
+      <c r="H36" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="4">
         <v>1</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="9">
-        <v>0</v>
-      </c>
-      <c r="F37" s="9">
+      <c r="E37" s="10">
+        <v>0</v>
+      </c>
+      <c r="F37" s="10">
         <v>0</v>
       </c>
       <c r="G37" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="10" t="s">
+      <c r="H37" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C38" s="4">
         <v>1</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="9">
-        <v>0</v>
-      </c>
-      <c r="F38" s="9">
+      <c r="E38" s="10">
+        <v>0</v>
+      </c>
+      <c r="F38" s="10">
         <v>0</v>
       </c>
       <c r="G38" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="10" t="s">
+      <c r="H38" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="4">
         <v>1</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E39" s="9">
-        <v>0</v>
-      </c>
-      <c r="F39" s="9">
+      <c r="E39" s="10">
+        <v>0</v>
+      </c>
+      <c r="F39" s="10">
         <v>0</v>
       </c>
       <c r="G39" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="10" t="s">
+      <c r="H39" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="4">
         <v>1</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E40" s="9">
-        <v>0</v>
-      </c>
-      <c r="F40" s="9">
+      <c r="E40" s="10">
+        <v>0</v>
+      </c>
+      <c r="F40" s="10">
         <v>0</v>
       </c>
       <c r="G40" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="10" t="s">
+      <c r="H40" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C41" s="4">
         <v>1</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="9">
-        <v>0</v>
-      </c>
-      <c r="F41" s="9">
+      <c r="E41" s="10">
+        <v>0</v>
+      </c>
+      <c r="F41" s="10">
         <v>0</v>
       </c>
       <c r="G41" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="10" t="s">
+      <c r="H41" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C42" s="4">
         <v>1</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E42" s="9">
-        <v>0</v>
-      </c>
-      <c r="F42" s="9">
+      <c r="E42" s="10">
+        <v>0</v>
+      </c>
+      <c r="F42" s="10">
         <v>0</v>
       </c>
       <c r="G42" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="10" t="s">
+      <c r="H42" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C43" s="4">
         <v>1</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E43" s="9">
-        <v>0</v>
-      </c>
-      <c r="F43" s="9">
+      <c r="E43" s="10">
+        <v>0</v>
+      </c>
+      <c r="F43" s="10">
         <v>0</v>
       </c>
       <c r="G43" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="10" t="s">
+      <c r="H43" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C44" s="4">
         <v>1</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="9">
-        <v>0</v>
-      </c>
-      <c r="F44" s="9">
+      <c r="E44" s="10">
+        <v>0</v>
+      </c>
+      <c r="F44" s="10">
         <v>0</v>
       </c>
       <c r="G44" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="10" t="s">
+      <c r="H44" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C45" s="4">
         <v>1</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E45" s="9">
-        <v>0</v>
-      </c>
-      <c r="F45" s="9">
+      <c r="E45" s="10">
+        <v>0</v>
+      </c>
+      <c r="F45" s="10">
         <v>0</v>
       </c>
       <c r="G45" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="10" t="s">
+      <c r="H45" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C46" s="4">
         <v>1</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E46" s="9">
-        <v>0</v>
-      </c>
-      <c r="F46" s="9">
+      <c r="E46" s="10">
+        <v>0</v>
+      </c>
+      <c r="F46" s="10">
         <v>0</v>
       </c>
       <c r="G46" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="10" t="s">
+      <c r="H46" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="4">
         <v>1</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E47" s="9">
-        <v>0</v>
-      </c>
-      <c r="F47" s="9">
+      <c r="E47" s="10">
+        <v>0</v>
+      </c>
+      <c r="F47" s="10">
         <v>0</v>
       </c>
       <c r="G47" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="10" t="s">
+      <c r="H47" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C48" s="4">
         <v>1</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E48" s="9">
-        <v>0</v>
-      </c>
-      <c r="F48" s="9">
+      <c r="E48" s="10">
+        <v>0</v>
+      </c>
+      <c r="F48" s="10">
         <v>0</v>
       </c>
       <c r="G48" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="10" t="s">
+      <c r="H48" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C49" s="4">
         <v>1</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E49" s="10">
         <v>16.3</v>
       </c>
-      <c r="F49" s="9">
+      <c r="F49" s="10">
         <v>53.5</v>
       </c>
       <c r="G49" s="7">
         <v>32</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="10" t="s">
+      <c r="H49" s="11">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C50" s="4">
         <v>1</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E50" s="9">
+      <c r="E50" s="10">
         <v>12.3</v>
       </c>
-      <c r="F50" s="9">
+      <c r="F50" s="10">
         <v>50.6</v>
       </c>
       <c r="G50" s="7">
         <v>97</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="10" t="s">
+      <c r="H50" s="11">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C51" s="4">
         <v>1</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E51" s="9">
+        <v>50</v>
+      </c>
+      <c r="E51" s="10">
         <v>12.7</v>
       </c>
-      <c r="F51" s="9">
+      <c r="F51" s="10">
         <v>51.2</v>
       </c>
       <c r="G51" s="7">
         <v>38</v>
       </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="10" t="s">
+      <c r="H51" s="11">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C52" s="4">
         <v>1</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E52" s="9">
+        <v>50</v>
+      </c>
+      <c r="E52" s="10">
         <v>13.2</v>
       </c>
-      <c r="F52" s="9">
+      <c r="F52" s="10">
         <v>53.4</v>
       </c>
       <c r="G52" s="7">
         <v>63</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="10" t="s">
+      <c r="H52" s="11">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="4">
         <v>1</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E53" s="9">
+      <c r="E53" s="10">
         <v>12.7</v>
       </c>
-      <c r="F53" s="9">
+      <c r="F53" s="10">
         <v>54.6</v>
       </c>
       <c r="G53" s="7">
         <v>58</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="10" t="s">
+      <c r="H53" s="11">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C54" s="4">
         <v>1</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E54" s="9">
+        <v>50</v>
+      </c>
+      <c r="E54" s="10">
         <v>12.7</v>
       </c>
-      <c r="F54" s="9">
+      <c r="F54" s="10">
         <v>51.1</v>
       </c>
       <c r="G54" s="7">
         <v>58</v>
       </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="10" t="s">
+      <c r="H54" s="11">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C55" s="4">
         <v>1</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E55" s="10">
         <v>9.1</v>
       </c>
-      <c r="F55" s="9">
+      <c r="F55" s="10">
         <v>35.9</v>
       </c>
       <c r="G55" s="7">
         <v>22</v>
       </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="10" t="s">
+      <c r="H55" s="11">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C56" s="4">
         <v>1</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E56" s="9">
+        <v>50</v>
+      </c>
+      <c r="E56" s="10">
         <v>10</v>
       </c>
-      <c r="F56" s="9">
+      <c r="F56" s="10">
         <v>32</v>
       </c>
       <c r="G56" s="7">
         <v>57</v>
       </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="10" t="s">
+      <c r="H56" s="11">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C57" s="4">
         <v>1</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E57" s="9">
+        <v>50</v>
+      </c>
+      <c r="E57" s="10">
         <v>12</v>
       </c>
-      <c r="F57" s="9">
+      <c r="F57" s="10">
         <v>35</v>
       </c>
       <c r="G57" s="7">
         <v>39</v>
       </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="10" t="s">
+      <c r="H57" s="11">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C58" s="4">
         <v>1</v>
       </c>
-      <c r="D58" s="8" t="s">
+      <c r="D58" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E58" s="9">
+      <c r="E58" s="10">
         <v>11</v>
       </c>
-      <c r="F58" s="9">
+      <c r="F58" s="10">
         <v>45</v>
       </c>
       <c r="G58" s="7">
         <v>62</v>
       </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="10" t="s">
+      <c r="H58" s="11">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C59" s="4">
         <v>1</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="D59" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E59" s="9">
+      <c r="E59" s="10">
         <v>9</v>
       </c>
-      <c r="F59" s="9">
+      <c r="F59" s="10">
         <v>50</v>
       </c>
       <c r="G59" s="7">
         <v>62.5</v>
       </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" s="10">
+      <c r="H59" s="11">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" s="12">
         <v>2</v>
       </c>
       <c r="D60" s="5" t="s">
@@ -1894,12 +2078,15 @@
       <c r="G60" s="7">
         <v>69</v>
       </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="10">
+      <c r="H60" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="12">
         <v>2</v>
       </c>
       <c r="D61" s="5" t="s">
@@ -1914,12 +2101,15 @@
       <c r="G61" s="7">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C62" s="10">
+      <c r="H61" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" s="12">
         <v>2</v>
       </c>
       <c r="D62" s="5" t="s">
@@ -1934,12 +2124,15 @@
       <c r="G62" s="7">
         <v>71</v>
       </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63" s="10">
+      <c r="H62" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" s="12">
         <v>2</v>
       </c>
       <c r="D63" s="5" t="s">
@@ -1954,12 +2147,15 @@
       <c r="G63" s="7">
         <v>16.2</v>
       </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C64" s="10">
+      <c r="H63" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64" s="12">
         <v>2</v>
       </c>
       <c r="D64" s="5" t="s">
@@ -1974,12 +2170,15 @@
       <c r="G64" s="7">
         <v>56</v>
       </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B65" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C65" s="10">
+      <c r="H64" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65" s="12">
         <v>2</v>
       </c>
       <c r="D65" s="5" t="s">
@@ -1994,12 +2193,15 @@
       <c r="G65" s="7">
         <v>95</v>
       </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B66" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C66" s="10">
+      <c r="H65" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" s="12">
         <v>2</v>
       </c>
       <c r="D66" s="5" t="s">
@@ -2011,15 +2213,18 @@
       <c r="F66" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G66" s="13">
+      <c r="G66" s="15">
         <v>62.5</v>
       </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B67" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C67" s="10">
+      <c r="H66" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C67" s="12">
         <v>2</v>
       </c>
       <c r="D67" s="5" t="s">
@@ -2031,15 +2236,18 @@
       <c r="F67" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G67" s="13">
+      <c r="G67" s="15">
         <v>90</v>
       </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B68" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C68" s="10">
+      <c r="H67" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68" s="12">
         <v>2</v>
       </c>
       <c r="D68" s="5" t="s">
@@ -2054,12 +2262,15 @@
       <c r="G68" s="7">
         <v>53</v>
       </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B69" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C69" s="10">
+      <c r="H68" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69" s="12">
         <v>2</v>
       </c>
       <c r="D69" s="5" t="s">
@@ -2074,12 +2285,15 @@
       <c r="G69" s="7">
         <v>78</v>
       </c>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C70" s="10">
+      <c r="H69" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" s="12">
         <v>2</v>
       </c>
       <c r="D70" s="5" t="s">
@@ -2094,12 +2308,15 @@
       <c r="G70" s="7">
         <v>73.5</v>
       </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C71" s="10">
+      <c r="H70" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71" s="12">
         <v>2</v>
       </c>
       <c r="D71" s="5" t="s">
@@ -2114,12 +2331,15 @@
       <c r="G71" s="7">
         <v>6.2</v>
       </c>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B72" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C72" s="10">
+      <c r="H71" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C72" s="12">
         <v>2</v>
       </c>
       <c r="D72" s="5" t="s">
@@ -2134,12 +2354,15 @@
       <c r="G72" s="7">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B73" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C73" s="10">
+      <c r="H72" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" s="12">
         <v>2</v>
       </c>
       <c r="D73" s="5" t="s">
@@ -2154,12 +2377,15 @@
       <c r="G73" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B74" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C74" s="10">
+      <c r="H73" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74" s="12">
         <v>2</v>
       </c>
       <c r="D74" s="5" t="s">
@@ -2174,12 +2400,15 @@
       <c r="G74" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B75" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C75" s="10">
+      <c r="H74" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C75" s="12">
         <v>2</v>
       </c>
       <c r="D75" s="5" t="s">
@@ -2194,12 +2423,15 @@
       <c r="G75" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B76" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C76" s="10">
+      <c r="H75" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76" s="12">
         <v>2</v>
       </c>
       <c r="D76" s="5" t="s">
@@ -2214,12 +2446,15 @@
       <c r="G76" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B77" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C77" s="10">
+      <c r="H76" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77" s="12">
         <v>2</v>
       </c>
       <c r="D77" s="5" t="s">
@@ -2234,12 +2469,15 @@
       <c r="G77" s="7">
         <v>7</v>
       </c>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C78" s="10">
+      <c r="H77" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C78" s="12">
         <v>2</v>
       </c>
       <c r="D78" s="5" t="s">
@@ -2254,12 +2492,15 @@
       <c r="G78" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C79" s="10">
+      <c r="H78" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C79" s="12">
         <v>2</v>
       </c>
       <c r="D79" s="5" t="s">
@@ -2274,12 +2515,15 @@
       <c r="G79" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C80" s="10">
+      <c r="H79" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="12">
         <v>2</v>
       </c>
       <c r="D80" s="5" t="s">
@@ -2294,12 +2538,15 @@
       <c r="G80" s="7">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B81" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C81" s="10">
+      <c r="H80" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C81" s="12">
         <v>2</v>
       </c>
       <c r="D81" s="5" t="s">
@@ -2314,12 +2561,15 @@
       <c r="G81" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B82" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C82" s="10">
+      <c r="H81" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C82" s="12">
         <v>2</v>
       </c>
       <c r="D82" s="5" t="s">
@@ -2334,15 +2584,18 @@
       <c r="G82" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B83" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C83" s="10">
-        <v>2</v>
-      </c>
-      <c r="D83" s="11" t="s">
+      <c r="H82" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83" s="12">
+        <v>2</v>
+      </c>
+      <c r="D83" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E83" s="6">
@@ -2354,15 +2607,18 @@
       <c r="G83" s="7">
         <v>84</v>
       </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B84" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C84" s="12">
-        <v>2</v>
-      </c>
-      <c r="D84" s="8" t="s">
+      <c r="H83" s="8">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C84" s="14">
+        <v>2</v>
+      </c>
+      <c r="D84" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E84" s="6">
@@ -2374,15 +2630,18 @@
       <c r="G84" s="7">
         <v>47</v>
       </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C85" s="10">
-        <v>2</v>
-      </c>
-      <c r="D85" s="11" t="s">
+      <c r="H84" s="8">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C85" s="12">
+        <v>2</v>
+      </c>
+      <c r="D85" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E85" s="6">
@@ -2394,15 +2653,18 @@
       <c r="G85" s="7">
         <v>78</v>
       </c>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C86" s="12">
-        <v>2</v>
-      </c>
-      <c r="D86" s="11" t="s">
+      <c r="H85" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C86" s="14">
+        <v>2</v>
+      </c>
+      <c r="D86" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E86" s="6">
@@ -2414,15 +2676,18 @@
       <c r="G86" s="7">
         <v>90</v>
       </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B87" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C87" s="10">
-        <v>2</v>
-      </c>
-      <c r="D87" s="11" t="s">
+      <c r="H86" s="8">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C87" s="12">
+        <v>2</v>
+      </c>
+      <c r="D87" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E87" s="6">
@@ -2434,12 +2699,15 @@
       <c r="G87" s="7">
         <v>62</v>
       </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B88" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C88" s="12">
+      <c r="H87" s="8">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C88" s="14">
         <v>2</v>
       </c>
       <c r="D88" s="7" t="s">
@@ -2454,12 +2722,15 @@
       <c r="G88" s="7">
         <v>60</v>
       </c>
-    </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C89" s="10">
+      <c r="H88" s="7">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C89" s="12">
         <v>2</v>
       </c>
       <c r="D89" s="7" t="s">
@@ -2474,15 +2745,18 @@
       <c r="G89" s="7">
         <v>22</v>
       </c>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B90" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C90" s="12">
-        <v>2</v>
-      </c>
-      <c r="D90" s="8" t="s">
+      <c r="H89" s="7">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C90" s="14">
+        <v>2</v>
+      </c>
+      <c r="D90" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E90" s="7">
@@ -2494,12 +2768,15 @@
       <c r="G90" s="7">
         <v>85</v>
       </c>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B91" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C91" s="10">
+      <c r="H90" s="7">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C91" s="12">
         <v>2</v>
       </c>
       <c r="D91" s="7" t="s">
@@ -2514,12 +2791,15 @@
       <c r="G91" s="7">
         <v>22</v>
       </c>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B92" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C92" s="12">
+      <c r="H91" s="7">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C92" s="14">
         <v>2</v>
       </c>
       <c r="D92" s="7" t="s">
@@ -2534,12 +2814,15 @@
       <c r="G92" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B93" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C93" s="10">
+      <c r="H92" s="7">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C93" s="12">
         <v>2</v>
       </c>
       <c r="D93" s="7" t="s">
@@ -2554,12 +2837,15 @@
       <c r="G93" s="7">
         <v>12</v>
       </c>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B94" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C94" s="12">
+      <c r="H93" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C94" s="14">
         <v>2</v>
       </c>
       <c r="D94" s="7" t="s">
@@ -2574,12 +2860,15 @@
       <c r="G94" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B95" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C95" s="10">
+      <c r="H94" s="7">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B95" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C95" s="12">
         <v>2</v>
       </c>
       <c r="D95" s="7" t="s">
@@ -2594,12 +2883,15 @@
       <c r="G95" s="7">
         <v>9</v>
       </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B96" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C96" s="12">
+      <c r="H95" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B96" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C96" s="14">
         <v>2</v>
       </c>
       <c r="D96" s="7" t="s">
@@ -2614,12 +2906,15 @@
       <c r="G96" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B97" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C97" s="10">
+      <c r="H96" s="7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C97" s="12">
         <v>2</v>
       </c>
       <c r="D97" s="7" t="s">
@@ -2634,12 +2929,15 @@
       <c r="G97" s="7">
         <v>7</v>
       </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C98" s="12">
+      <c r="H97" s="7">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C98" s="14">
         <v>2</v>
       </c>
       <c r="D98" s="7" t="s">
@@ -2654,12 +2952,15 @@
       <c r="G98" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B99" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C99" s="10">
+      <c r="H98" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C99" s="12">
         <v>2</v>
       </c>
       <c r="D99" s="7" t="s">
@@ -2674,12 +2975,15 @@
       <c r="G99" s="7">
         <v>9</v>
       </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B100" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C100" s="12">
+      <c r="H99" s="7">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C100" s="14">
         <v>2</v>
       </c>
       <c r="D100" s="7" t="s">
@@ -2694,12 +2998,15 @@
       <c r="G100" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B101" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C101" s="10">
+      <c r="H100" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C101" s="12">
         <v>2</v>
       </c>
       <c r="D101" s="7" t="s">
@@ -2714,12 +3021,15 @@
       <c r="G101" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B102" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C102" s="12">
+      <c r="H101" s="7">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C102" s="14">
         <v>2</v>
       </c>
       <c r="D102" s="7" t="s">
@@ -2734,15 +3044,18 @@
       <c r="G102" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B103" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C103" s="10">
-        <v>2</v>
-      </c>
-      <c r="D103" s="11" t="s">
+      <c r="H102" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B103" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C103" s="12">
+        <v>2</v>
+      </c>
+      <c r="D103" s="13" t="s">
         <v>39</v>
       </c>
       <c r="E103" s="6">
@@ -2754,15 +3067,18 @@
       <c r="G103" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B104" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C104" s="10">
+      <c r="H103" s="8">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B104" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C104" s="12">
         <v>3</v>
       </c>
-      <c r="D104" s="8" t="s">
+      <c r="D104" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E104" s="6">
@@ -2774,15 +3090,18 @@
       <c r="G104" s="7">
         <v>68</v>
       </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B105" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C105" s="10">
+      <c r="H104" s="8">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C105" s="12">
         <v>3</v>
       </c>
-      <c r="D105" s="11" t="s">
+      <c r="D105" s="13" t="s">
         <v>39</v>
       </c>
       <c r="E105" s="6">
@@ -2794,15 +3113,18 @@
       <c r="G105" s="7">
         <v>29</v>
       </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B106" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C106" s="10">
+      <c r="H105" s="8">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B106" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C106" s="12">
         <v>3</v>
       </c>
-      <c r="D106" s="11" t="s">
+      <c r="D106" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E106" s="6">
@@ -2814,15 +3136,18 @@
       <c r="G106" s="7">
         <v>130</v>
       </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C107" s="10">
+      <c r="H106" s="8">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B107" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C107" s="12">
         <v>3</v>
       </c>
-      <c r="D107" s="8" t="s">
+      <c r="D107" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E107" s="6">
@@ -2834,15 +3159,18 @@
       <c r="G107" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B108" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C108" s="10">
+      <c r="H107" s="8">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B108" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C108" s="12">
         <v>3</v>
       </c>
-      <c r="D108" s="8" t="s">
+      <c r="D108" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E108" s="6">
@@ -2854,15 +3182,18 @@
       <c r="G108" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B109" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C109" s="10">
+      <c r="H108" s="8">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B109" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C109" s="12">
         <v>3</v>
       </c>
-      <c r="D109" s="11" t="s">
+      <c r="D109" s="13" t="s">
         <v>41</v>
       </c>
       <c r="E109" s="6">
@@ -2874,15 +3205,18 @@
       <c r="G109" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B110" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C110" s="10">
+      <c r="H109" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B110" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C110" s="12">
         <v>3</v>
       </c>
-      <c r="D110" s="11" t="s">
+      <c r="D110" s="13" t="s">
         <v>42</v>
       </c>
       <c r="E110" s="6">
@@ -2894,15 +3228,18 @@
       <c r="G110" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B111" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C111" s="10">
+      <c r="H110" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B111" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C111" s="12">
         <v>3</v>
       </c>
-      <c r="D111" s="11" t="s">
+      <c r="D111" s="13" t="s">
         <v>43</v>
       </c>
       <c r="E111" s="6">
@@ -2914,15 +3251,18 @@
       <c r="G111" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B112" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C112" s="10">
+      <c r="H111" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B112" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C112" s="12">
         <v>3</v>
       </c>
-      <c r="D112" s="11" t="s">
+      <c r="D112" s="13" t="s">
         <v>36</v>
       </c>
       <c r="E112" s="6">
@@ -2934,12 +3274,15 @@
       <c r="G112" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B113" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C113" s="10">
+      <c r="H112" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B113" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C113" s="12">
         <v>3</v>
       </c>
       <c r="D113" s="5" t="s">
@@ -2954,12 +3297,15 @@
       <c r="G113" s="7">
         <v>58</v>
       </c>
-    </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B114" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C114" s="10">
+      <c r="H113" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B114" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C114" s="12">
         <v>3</v>
       </c>
       <c r="D114" s="5" t="s">
@@ -2974,12 +3320,15 @@
       <c r="G114" s="7">
         <v>54</v>
       </c>
-    </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B115" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C115" s="10">
+      <c r="H114" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B115" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C115" s="12">
         <v>3</v>
       </c>
       <c r="D115" s="5" t="s">
@@ -2994,12 +3343,15 @@
       <c r="G115" s="7">
         <v>71</v>
       </c>
-    </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C116" s="10">
+      <c r="H115" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B116" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C116" s="12">
         <v>3</v>
       </c>
       <c r="D116" s="5" t="s">
@@ -3014,12 +3366,15 @@
       <c r="G116" s="7">
         <v>71.5</v>
       </c>
-    </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B117" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C117" s="10">
+      <c r="H116" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B117" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C117" s="12">
         <v>3</v>
       </c>
       <c r="D117" s="5" t="s">
@@ -3034,12 +3389,15 @@
       <c r="G117" s="7">
         <v>61.5</v>
       </c>
-    </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B118" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C118" s="10">
+      <c r="H117" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B118" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C118" s="12">
         <v>3</v>
       </c>
       <c r="D118" s="5" t="s">
@@ -3054,12 +3412,15 @@
       <c r="G118" s="7">
         <v>55.5</v>
       </c>
-    </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B119" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C119" s="10">
+      <c r="H118" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B119" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C119" s="12">
         <v>3</v>
       </c>
       <c r="D119" s="5" t="s">
@@ -3074,12 +3435,15 @@
       <c r="G119" s="7">
         <v>35</v>
       </c>
-    </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B120" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C120" s="10">
+      <c r="H119" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B120" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C120" s="12">
         <v>3</v>
       </c>
       <c r="D120" s="5" t="s">
@@ -3094,12 +3458,15 @@
       <c r="G120" s="7">
         <v>47</v>
       </c>
-    </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B121" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C121" s="10">
+      <c r="H120" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B121" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C121" s="12">
         <v>3</v>
       </c>
       <c r="D121" s="5" t="s">
@@ -3114,12 +3481,15 @@
       <c r="G121" s="7">
         <v>42.5</v>
       </c>
-    </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B122" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C122" s="10">
+      <c r="H121" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B122" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C122" s="12">
         <v>3</v>
       </c>
       <c r="D122" s="5" t="s">
@@ -3134,12 +3504,15 @@
       <c r="G122" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B123" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C123" s="10">
+      <c r="H122" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B123" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C123" s="12">
         <v>3</v>
       </c>
       <c r="D123" s="5" t="s">
@@ -3154,12 +3527,15 @@
       <c r="G123" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B124" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C124" s="10">
+      <c r="H123" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B124" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C124" s="12">
         <v>3</v>
       </c>
       <c r="D124" s="5" t="s">
@@ -3174,12 +3550,15 @@
       <c r="G124" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C125" s="10">
+      <c r="H124" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B125" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C125" s="12">
         <v>3</v>
       </c>
       <c r="D125" s="5" t="s">
@@ -3194,16 +3573,19 @@
       <c r="G125" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B126" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C126" s="10">
+      <c r="H125" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B126" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C126" s="12">
         <v>3</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E126" s="6">
         <v>15</v>
@@ -3214,16 +3596,19 @@
       <c r="G126" s="7">
         <v>19</v>
       </c>
-    </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B127" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C127" s="10">
+      <c r="H126" s="8">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B127" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C127" s="12">
         <v>3</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E127" s="6">
         <v>15</v>
@@ -3234,9 +3619,12 @@
       <c r="G127" s="7">
         <v>22.5</v>
       </c>
+      <c r="H127" s="8">
+        <v>0.7</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:G127" xr:uid="{0C545A6F-2989-4DB9-8EDF-13C16FDF8F37}"/>
+  <autoFilter ref="B2:H127" xr:uid="{0C545A6F-2989-4DB9-8EDF-13C16FDF8F37}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>